<commit_message>
Added BOM for hardware schematics.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="158">
   <si>
     <t>Manufacturer ID</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>67R8591</t>
+  </si>
+  <si>
+    <t>BOM for Nucleon Shield.</t>
   </si>
 </sst>
 </file>
@@ -903,11 +906,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -918,6 +919,11 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>

</xml_diff>